<commit_message>
Change folder for reserves file
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_IT.xlsx
+++ b/ConfigFiles/Config_IT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfranssens/Dispa-SET.git/ConfigFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiara Magni\Desktop\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8532B590-F77B-3F4E-9228-DBEDF205FA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E18F73-4FB4-4D8E-A897-FFAFF53D9A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="221">
   <si>
     <t>Default value</t>
   </si>
@@ -695,10 +695,7 @@
     <t>Database/Heat_demand/2016.csv</t>
   </si>
   <si>
-    <t>Database/Reserves/up/##/OSE_ReserveDemand_2019.csv</t>
-  </si>
-  <si>
-    <t>Database/Reserves/down/##/OSE_ReserveDemand_2019.csv</t>
+    <t>Database\Reserves\reserves_probabilistic.csv</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1008,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1079,7 +1076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1402,24 +1399,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="C307" sqref="C307"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>195</v>
       </c>
@@ -1431,7 +1428,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1441,8 +1438,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
         <v>57</v>
@@ -1454,7 +1451,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1464,7 +1461,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
@@ -1478,7 +1475,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -1487,7 +1484,7 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
@@ -1496,7 +1493,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -1505,7 +1502,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1514,7 +1511,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -1523,7 +1520,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -1532,7 +1529,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -1541,7 +1538,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
     </row>
-    <row r="14" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1550,7 +1547,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>179</v>
       </c>
@@ -1562,39 +1559,39 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="29"/>
     </row>
-    <row r="17" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="30"/>
     </row>
-    <row r="18" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>169</v>
       </c>
@@ -1606,7 +1603,7 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1621,7 +1618,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1635,7 +1632,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1649,7 +1646,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -1660,7 +1657,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>131</v>
       </c>
@@ -1672,24 +1669,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>168</v>
       </c>
@@ -1701,7 +1698,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1715,7 +1712,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -1729,7 +1726,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -1743,7 +1740,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>48</v>
       </c>
@@ -1754,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>199</v>
       </c>
@@ -1765,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>200</v>
       </c>
@@ -1776,19 +1773,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>166</v>
       </c>
@@ -1800,10 +1797,10 @@
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>42</v>
       </c>
@@ -1817,7 +1814,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -1831,7 +1828,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -1845,76 +1842,76 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>173</v>
       </c>
@@ -1926,7 +1923,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>140</v>
       </c>
@@ -1940,7 +1937,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>162</v>
       </c>
@@ -1954,7 +1951,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>176</v>
       </c>
@@ -1965,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
         <v>174</v>
       </c>
@@ -1979,7 +1976,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
         <v>175</v>
       </c>
@@ -1993,30 +1990,30 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
         <v>167</v>
       </c>
@@ -2028,7 +2025,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="36"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2043,7 +2040,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>193</v>
       </c>
@@ -2062,7 +2059,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2079,7 +2076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2096,7 +2093,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>37</v>
       </c>
@@ -2110,7 +2107,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>41</v>
       </c>
@@ -2131,7 +2128,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>49</v>
       </c>
@@ -2148,7 +2145,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>90</v>
       </c>
@@ -2165,7 +2162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>128</v>
       </c>
@@ -2182,7 +2179,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -2196,7 +2193,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
@@ -2210,7 +2207,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -2223,103 +2220,103 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="25"/>
       <c r="C137" s="27"/>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="C138" s="27"/>
     </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25"/>
       <c r="C139" s="27"/>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
       <c r="C140" s="27"/>
     </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
       <c r="C141" s="27"/>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="C142" s="27"/>
     </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
         <v>210</v>
       </c>
@@ -2330,7 +2327,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
         <v>209</v>
       </c>
@@ -2338,10 +2335,10 @@
         <v>36</v>
       </c>
       <c r="C162" s="19" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>204</v>
       </c>
@@ -2356,7 +2353,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>202</v>
       </c>
@@ -2370,11 +2367,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
       <c r="C165" s="27"/>
     </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
         <v>192</v>
       </c>
@@ -2386,7 +2383,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="36"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>124</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
@@ -2422,7 +2419,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2443,7 +2440,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -2464,47 +2461,47 @@
         <v>208</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25"/>
       <c r="C171" s="27"/>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>122</v>
       </c>
@@ -2520,7 +2517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>91</v>
       </c>
@@ -2540,7 +2537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -2563,7 +2560,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>63</v>
       </c>
@@ -2583,7 +2580,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>123</v>
       </c>
@@ -2603,7 +2600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>129</v>
       </c>
@@ -2621,7 +2618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>130</v>
       </c>
@@ -2639,66 +2636,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25"/>
       <c r="C188" s="27"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="25"/>
       <c r="C192" s="27"/>
     </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="25"/>
       <c r="C193" s="27"/>
     </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
     </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="25"/>
       <c r="C195" s="27"/>
     </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="25"/>
       <c r="C196" s="27"/>
     </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="25"/>
       <c r="C197" s="27"/>
     </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="25"/>
       <c r="C198" s="27"/>
     </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="25"/>
       <c r="C199" s="27"/>
     </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="25"/>
       <c r="C200" s="27"/>
     </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="25"/>
       <c r="C201" s="27"/>
     </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="25"/>
       <c r="C202" s="27"/>
     </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="25"/>
       <c r="C203" s="27"/>
     </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>147</v>
       </c>
@@ -2713,7 +2710,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>145</v>
       </c>
@@ -2728,7 +2725,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2743,71 +2740,71 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="25"/>
       <c r="C209" s="27"/>
     </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="25"/>
       <c r="C210" s="27"/>
     </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
         <v>170</v>
       </c>
@@ -2831,7 +2828,7 @@
       </c>
       <c r="H225" s="40"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>51</v>
       </c>
@@ -2854,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="47" t="s">
         <v>52</v>
       </c>
@@ -2877,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>22</v>
@@ -2898,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>15</v>
@@ -2919,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>134</v>
@@ -2940,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -2961,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>154</v>
@@ -2982,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>31</v>
@@ -3003,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3024,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3045,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3066,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3087,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3108,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3129,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3150,7 +3147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>28</v>
@@ -3171,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3191,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3211,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
         <v>20</v>
       </c>
@@ -3231,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="50" t="s">
         <v>172</v>
       </c>
@@ -3254,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>160</v>
@@ -3278,7 +3275,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3298,108 +3295,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="35" t="s">
         <v>73</v>
       </c>
@@ -3411,7 +3408,7 @@
       <c r="G274" s="36"/>
       <c r="H274" s="36"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3422,7 +3419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>74</v>
       </c>
@@ -3436,7 +3433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>75</v>
       </c>
@@ -3450,7 +3447,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>77</v>
       </c>
@@ -3461,35 +3458,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="9"/>
       <c r="C302" s="14"/>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="39" t="s">
         <v>171</v>
       </c>
@@ -3501,7 +3498,7 @@
       <c r="G304" s="40"/>
       <c r="H304" s="40"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>121</v>
       </c>
@@ -3509,7 +3506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
         <v>92</v>
       </c>
@@ -3517,7 +3514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
         <v>93</v>
       </c>
@@ -3525,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
         <v>94</v>
       </c>
@@ -3533,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
         <v>95</v>
       </c>
@@ -3541,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
         <v>96</v>
       </c>
@@ -3549,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
         <v>97</v>
       </c>
@@ -3557,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
         <v>98</v>
       </c>
@@ -3565,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
         <v>99</v>
       </c>
@@ -3573,7 +3570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
         <v>100</v>
       </c>
@@ -3581,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
         <v>101</v>
       </c>
@@ -3589,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
         <v>102</v>
       </c>
@@ -3597,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
         <v>103</v>
       </c>
@@ -3605,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
         <v>104</v>
       </c>
@@ -3613,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
         <v>105</v>
       </c>
@@ -3621,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
         <v>106</v>
       </c>
@@ -3629,12 +3626,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3781,16 +3778,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3830,7 +3827,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3847,7 +3844,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -3858,7 +3855,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -3866,7 +3863,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3882,16 +3879,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
@@ -3935,7 +3932,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -3982,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>94</v>
       </c>
@@ -4076,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
@@ -4123,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
@@ -4170,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>97</v>
       </c>
@@ -4217,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
@@ -4264,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>99</v>
       </c>
@@ -4311,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>100</v>
       </c>
@@ -4358,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -4405,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -4452,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
@@ -4499,7 +4496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>104</v>
       </c>
@@ -4546,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>105</v>
       </c>
@@ -4593,7 +4590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
option to chose which technology with or without CHP can participate in the reserve market
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_IT.xlsx
+++ b/ConfigFiles/Config_IT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiara Magni\Desktop\Dispa-SET.git\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfranssens/Dispa-SET.git/ConfigFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E18F73-4FB4-4D8E-A897-FFAFF53D9A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E60E699-753B-4C4E-8602-365E2BB079E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="223">
   <si>
     <t>Default value</t>
   </si>
@@ -695,7 +695,13 @@
     <t>Database/Heat_demand/2016.csv</t>
   </si>
   <si>
-    <t>Database\Reserves\reserves_probabilistic.csv</t>
+    <t>Database/Reserves/reserves_probabilistic.csv</t>
+  </si>
+  <si>
+    <t>True/False with CHP</t>
+  </si>
+  <si>
+    <t>True/False without CHP</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1014,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1076,7 +1082,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1399,24 +1405,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="C319" sqref="C319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>195</v>
       </c>
@@ -1428,7 +1434,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1438,8 +1444,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
         <v>57</v>
@@ -1451,7 +1457,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1461,7 +1467,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
@@ -1475,7 +1481,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -1484,7 +1490,7 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
@@ -1493,7 +1499,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -1502,7 +1508,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1511,7 +1517,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -1520,7 +1526,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -1529,7 +1535,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -1538,7 +1544,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
     </row>
-    <row r="14" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1547,7 +1553,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>179</v>
       </c>
@@ -1559,39 +1565,39 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="29"/>
     </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="30"/>
     </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
         <v>169</v>
       </c>
@@ -1603,7 +1609,7 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>131</v>
       </c>
@@ -1669,24 +1675,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="35" t="s">
         <v>168</v>
       </c>
@@ -1698,7 +1704,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>48</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>199</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>200</v>
       </c>
@@ -1773,19 +1779,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="35" t="s">
         <v>166</v>
       </c>
@@ -1797,10 +1803,10 @@
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>42</v>
       </c>
@@ -1814,7 +1820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -1842,76 +1848,76 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="35" t="s">
         <v>173</v>
       </c>
@@ -1923,7 +1929,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>140</v>
       </c>
@@ -1937,7 +1943,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>162</v>
       </c>
@@ -1951,7 +1957,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>176</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="32" t="s">
         <v>174</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="32" t="s">
         <v>175</v>
       </c>
@@ -1990,30 +1996,30 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="35" t="s">
         <v>167</v>
       </c>
@@ -2025,7 +2031,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="36"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2046,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>193</v>
       </c>
@@ -2059,7 +2065,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>37</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>41</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>49</v>
       </c>
@@ -2145,7 +2151,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>90</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>128</v>
       </c>
@@ -2179,7 +2185,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -2193,7 +2199,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -2220,103 +2226,103 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="25"/>
       <c r="C137" s="27"/>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="25"/>
       <c r="C138" s="27"/>
     </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="25"/>
       <c r="C139" s="27"/>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="25"/>
       <c r="C140" s="27"/>
     </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="25"/>
       <c r="C141" s="27"/>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="25"/>
       <c r="C142" s="27"/>
     </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="25" t="s">
         <v>210</v>
       </c>
@@ -2327,7 +2333,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="25" t="s">
         <v>209</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>204</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>202</v>
       </c>
@@ -2367,11 +2373,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="25"/>
       <c r="C165" s="27"/>
     </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="35" t="s">
         <v>192</v>
       </c>
@@ -2383,7 +2389,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="36"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>124</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
@@ -2419,7 +2425,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -2461,47 +2467,47 @@
         <v>208</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="25"/>
       <c r="C171" s="27"/>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>122</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>91</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -2560,7 +2566,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>63</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>123</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>129</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>130</v>
       </c>
@@ -2636,66 +2642,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="25"/>
       <c r="C188" s="27"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="25"/>
       <c r="C192" s="27"/>
     </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="25"/>
       <c r="C193" s="27"/>
     </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
     </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="25"/>
       <c r="C195" s="27"/>
     </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="25"/>
       <c r="C196" s="27"/>
     </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="25"/>
       <c r="C197" s="27"/>
     </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="25"/>
       <c r="C198" s="27"/>
     </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="25"/>
       <c r="C199" s="27"/>
     </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="25"/>
       <c r="C200" s="27"/>
     </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="25"/>
       <c r="C201" s="27"/>
     </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="25"/>
       <c r="C202" s="27"/>
     </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="25"/>
       <c r="C203" s="27"/>
     </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>147</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>145</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2740,71 +2746,71 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="25"/>
       <c r="C209" s="27"/>
     </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="25"/>
       <c r="C210" s="27"/>
     </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="39" t="s">
         <v>170</v>
       </c>
@@ -2828,7 +2834,7 @@
       </c>
       <c r="H225" s="40"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>51</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="47" t="s">
         <v>52</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>22</v>
@@ -2895,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>15</v>
@@ -2916,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>134</v>
@@ -2937,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -2958,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>154</v>
@@ -2979,13 +2985,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C233" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D233" s="4" t="b">
         <v>0</v>
@@ -3000,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3021,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3042,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3063,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3084,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3105,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3126,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3147,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>28</v>
@@ -3168,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B244" s="6" t="s">
         <v>20</v>
       </c>
@@ -3228,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="50" t="s">
         <v>172</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>160</v>
@@ -3275,7 +3281,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3295,108 +3301,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="35" t="s">
         <v>73</v>
       </c>
@@ -3408,7 +3414,7 @@
       <c r="G274" s="36"/>
       <c r="H274" s="36"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
         <v>74</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>75</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
         <v>77</v>
       </c>
@@ -3458,35 +3464,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="9"/>
       <c r="C302" s="14"/>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="304" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="39" t="s">
         <v>171</v>
       </c>
@@ -3498,140 +3504,188 @@
       <c r="G304" s="40"/>
       <c r="H304" s="40"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C305" s="31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="D305" s="31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B306" s="22" t="s">
         <v>92</v>
       </c>
       <c r="C306" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D306" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B307" s="22" t="s">
         <v>93</v>
       </c>
       <c r="C307" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D307" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B308" s="22" t="s">
         <v>94</v>
       </c>
       <c r="C308" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D308" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B309" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C309" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D309" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B310" s="22" t="s">
         <v>96</v>
       </c>
       <c r="C310" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D310" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B311" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C311" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D311" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B312" s="22" t="s">
         <v>98</v>
       </c>
       <c r="C312" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D312" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B313" s="22" t="s">
         <v>99</v>
       </c>
       <c r="C313" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D313" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B314" s="22" t="s">
         <v>100</v>
       </c>
       <c r="C314" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D314" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B315" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C315" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D315" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B316" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C316" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D316" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B317" s="22" t="s">
         <v>103</v>
       </c>
       <c r="C317" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D317" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B318" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C318" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D318" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B319" s="22" t="s">
         <v>105</v>
       </c>
       <c r="C319" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D319" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B320" s="22" t="s">
         <v>106</v>
       </c>
       <c r="C320" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D320" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3643,7 +3697,7 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:C320">
+  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:D320">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
@@ -3713,7 +3767,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C226:D247 F226:G247 C306:C320</xm:sqref>
+          <xm:sqref>C226:D247 F226:G247 C306:D320</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
@@ -3778,16 +3832,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3807,7 +3861,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3827,7 +3881,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3844,7 +3898,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -3855,7 +3909,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -3863,7 +3917,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3883,12 +3937,12 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
@@ -3932,7 +3986,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -3979,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -4026,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>94</v>
       </c>
@@ -4073,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
@@ -4120,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
@@ -4167,7 +4221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>97</v>
       </c>
@@ -4214,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
@@ -4261,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>99</v>
       </c>
@@ -4308,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>100</v>
       </c>
@@ -4355,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -4402,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -4449,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
@@ -4496,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>104</v>
       </c>
@@ -4543,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>105</v>
       </c>
@@ -4590,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
adding p2h technology for the reserve participation option
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_IT.xlsx
+++ b/ConfigFiles/Config_IT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfranssens/Dispa-SET.git/ConfigFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E60E699-753B-4C4E-8602-365E2BB079E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C57F07-0FA4-7841-8300-192FB426FA36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="224">
   <si>
     <t>Default value</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>True/False without CHP</t>
+  </si>
+  <si>
+    <t>P2HT</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1409,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+      <selection activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3680,6 +3683,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B321" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D321" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
         <v>206</v>
@@ -3697,7 +3711,7 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:D320">
+  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:D321">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
@@ -3767,7 +3781,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C226:D247 F226:G247 C306:D320</xm:sqref>
+          <xm:sqref>C226:D247 F226:G247 C306:D321</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Changed reserve participation for CHP in the config file
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_IT.xlsx
+++ b/ConfigFiles/Config_IT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfranssens/Dispa-SET.git/ConfigFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C57F07-0FA4-7841-8300-192FB426FA36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96C860B-B204-406A-B4AF-F3F726AE2F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="236">
   <si>
     <t>Default value</t>
   </si>
@@ -653,9 +653,6 @@
     <t>Number of equivalent storage hours for the flexibile demand</t>
   </si>
   <si>
-    <t>End of the Config file. This must be line number 325!</t>
-  </si>
-  <si>
     <t>Price of Transmission</t>
   </si>
   <si>
@@ -698,13 +695,52 @@
     <t>Database/Reserves/reserves_probabilistic.csv</t>
   </si>
   <si>
-    <t>True/False with CHP</t>
-  </si>
-  <si>
-    <t>True/False without CHP</t>
-  </si>
-  <si>
     <t>P2HT</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Probabilistic</t>
+  </si>
+  <si>
+    <t>Exogenous</t>
+  </si>
+  <si>
+    <t>End of the Config file. This must be line number 400</t>
+  </si>
+  <si>
+    <t>ICEN units without CHP</t>
+  </si>
+  <si>
+    <t>STUR units without CHP</t>
+  </si>
+  <si>
+    <t>COMC units without CHP</t>
+  </si>
+  <si>
+    <t>GTUR units without CHP</t>
+  </si>
+  <si>
+    <t>SCSP</t>
+  </si>
+  <si>
+    <t>COMC units with CHP</t>
+  </si>
+  <si>
+    <t>GTUR units with CHP</t>
+  </si>
+  <si>
+    <t>ICEN units with CHP</t>
+  </si>
+  <si>
+    <t>STUR units with CHP</t>
+  </si>
+  <si>
+    <t>(CHP units)</t>
+  </si>
+  <si>
+    <t>(Non-CHP units)</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1055,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1406,26 +1456,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="D326" sqref="D326"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="E318" sqref="E318"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>195</v>
       </c>
@@ -1437,7 +1487,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1447,8 +1497,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
         <v>57</v>
@@ -1460,7 +1510,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1470,7 +1520,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
@@ -1484,7 +1534,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -1493,7 +1543,7 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
@@ -1502,7 +1552,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -1511,7 +1561,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1520,7 +1570,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -1529,7 +1579,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -1538,7 +1588,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -1547,7 +1597,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
     </row>
-    <row r="14" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1556,7 +1606,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>179</v>
       </c>
@@ -1568,39 +1618,39 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="29"/>
     </row>
-    <row r="17" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="30"/>
     </row>
-    <row r="18" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>169</v>
       </c>
@@ -1612,7 +1662,7 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1627,7 +1677,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1641,7 +1691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1655,7 +1705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -1666,7 +1716,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>131</v>
       </c>
@@ -1678,24 +1728,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>168</v>
       </c>
@@ -1707,7 +1757,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1721,7 +1771,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -1735,7 +1785,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1799,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>48</v>
       </c>
@@ -1760,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>199</v>
       </c>
@@ -1771,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>200</v>
       </c>
@@ -1782,19 +1832,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>166</v>
       </c>
@@ -1806,10 +1856,10 @@
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>42</v>
       </c>
@@ -1823,7 +1873,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -1837,7 +1887,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -1851,76 +1901,76 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>173</v>
       </c>
@@ -1932,7 +1982,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>140</v>
       </c>
@@ -1946,7 +1996,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>162</v>
       </c>
@@ -1960,7 +2010,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>176</v>
       </c>
@@ -1971,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
         <v>174</v>
       </c>
@@ -1985,7 +2035,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
         <v>175</v>
       </c>
@@ -1999,30 +2049,30 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
         <v>167</v>
       </c>
@@ -2034,7 +2084,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="36"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2042,14 +2092,14 @@
         <v>36</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>89</v>
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>193</v>
       </c>
@@ -2068,7 +2118,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2076,7 +2126,7 @@
         <v>36</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D127" s="18" t="s">
         <v>89</v>
@@ -2085,7 +2135,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2093,7 +2143,7 @@
         <v>36</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>89</v>
@@ -2102,7 +2152,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>37</v>
       </c>
@@ -2110,13 +2160,13 @@
         <v>36</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>41</v>
       </c>
@@ -2137,7 +2187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>49</v>
       </c>
@@ -2145,7 +2195,7 @@
         <v>36</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>89</v>
@@ -2154,7 +2204,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>90</v>
       </c>
@@ -2162,7 +2212,7 @@
         <v>36</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D132" s="18" t="s">
         <v>89</v>
@@ -2171,7 +2221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>128</v>
       </c>
@@ -2179,7 +2229,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>89</v>
@@ -2188,7 +2238,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -2196,13 +2246,13 @@
         <v>36</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D134" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
@@ -2210,13 +2260,13 @@
         <v>36</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -2229,125 +2279,125 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="25"/>
       <c r="C137" s="27"/>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="C138" s="27"/>
     </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25"/>
       <c r="C139" s="27"/>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
       <c r="C140" s="27"/>
     </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
       <c r="C141" s="27"/>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="C142" s="27"/>
     </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B161" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B162" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C162" s="19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>204</v>
       </c>
@@ -2362,7 +2412,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>202</v>
       </c>
@@ -2376,11 +2426,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
       <c r="C165" s="27"/>
     </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
         <v>192</v>
       </c>
@@ -2392,7 +2442,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="36"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>124</v>
       </c>
@@ -2410,7 +2460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
@@ -2428,7 +2478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2449,9 +2499,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>36</v>
@@ -2467,50 +2517,50 @@
         <v>0</v>
       </c>
       <c r="H170" s="26" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25"/>
       <c r="C171" s="27"/>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>122</v>
       </c>
@@ -2526,7 +2576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>91</v>
       </c>
@@ -2546,7 +2596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -2569,7 +2619,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>63</v>
       </c>
@@ -2589,7 +2639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>123</v>
       </c>
@@ -2609,7 +2659,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>129</v>
       </c>
@@ -2627,7 +2677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>130</v>
       </c>
@@ -2645,66 +2695,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" s="26" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25"/>
       <c r="C188" s="27"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="25"/>
       <c r="C192" s="27"/>
     </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="25"/>
       <c r="C193" s="27"/>
     </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
     </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="25"/>
       <c r="C195" s="27"/>
     </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="25"/>
       <c r="C196" s="27"/>
     </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="25"/>
       <c r="C197" s="27"/>
     </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="25"/>
       <c r="C198" s="27"/>
     </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="25"/>
       <c r="C199" s="27"/>
     </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="25"/>
       <c r="C200" s="27"/>
     </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="25"/>
       <c r="C201" s="27"/>
     </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="25"/>
       <c r="C202" s="27"/>
     </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="25"/>
       <c r="C203" s="27"/>
     </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>147</v>
       </c>
@@ -2719,7 +2769,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>145</v>
       </c>
@@ -2734,7 +2784,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2749,71 +2799,71 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="25"/>
       <c r="C209" s="27"/>
     </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="25"/>
       <c r="C210" s="27"/>
     </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
         <v>170</v>
       </c>
@@ -2837,7 +2887,7 @@
       </c>
       <c r="H225" s="40"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>51</v>
       </c>
@@ -2860,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="47" t="s">
         <v>52</v>
       </c>
@@ -2883,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>22</v>
@@ -2904,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>15</v>
@@ -2925,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>134</v>
@@ -2946,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -2967,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>154</v>
@@ -2988,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>31</v>
@@ -3009,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3030,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3051,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3072,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3093,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3114,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3135,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3156,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>28</v>
@@ -3177,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3197,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3217,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
         <v>20</v>
       </c>
@@ -3237,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="50" t="s">
         <v>172</v>
       </c>
@@ -3260,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>160</v>
@@ -3284,7 +3334,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3304,108 +3354,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="38" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="35" t="s">
         <v>73</v>
       </c>
@@ -3417,7 +3467,7 @@
       <c r="G274" s="36"/>
       <c r="H274" s="36"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3428,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>74</v>
       </c>
@@ -3442,7 +3492,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>75</v>
       </c>
@@ -3456,7 +3506,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>77</v>
       </c>
@@ -3467,35 +3517,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="1:8" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="9"/>
       <c r="C302" s="14"/>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="1:8" s="41" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="39" t="s">
         <v>171</v>
       </c>
@@ -3507,200 +3557,271 @@
       <c r="G304" s="40"/>
       <c r="H304" s="40"/>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C305" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="D305" s="31" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="B306" s="22" t="s">
         <v>92</v>
       </c>
       <c r="C306" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D306" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D306" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
         <v>93</v>
       </c>
       <c r="C307" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D307" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D307" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
         <v>94</v>
       </c>
       <c r="C308" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D308" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C309" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D309" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
         <v>96</v>
       </c>
       <c r="C310" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D310" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C311" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D311" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D311" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
         <v>98</v>
       </c>
       <c r="C312" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D312" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
         <v>99</v>
       </c>
       <c r="C313" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="D313" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D313" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
         <v>100</v>
       </c>
       <c r="C314" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D314" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C315" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="D315" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C316" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D316" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
         <v>103</v>
       </c>
       <c r="C317" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D317" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C318" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D318" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
         <v>105</v>
       </c>
       <c r="C319" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D319" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
         <v>106</v>
       </c>
       <c r="C320" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D320" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="321" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C321" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D321" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A325" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F330" s="2"/>
+    </row>
+    <row r="322" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B322" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C322" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="324" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="325" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="326" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="327" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="328" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="329" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="330" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="331" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F331" s="2"/>
+    </row>
+    <row r="332" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="333" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="334" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="335" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="336" spans="2:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="337" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="338" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="339" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C342" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B343" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C343" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B344" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C344" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B345" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C345" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B346" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C346" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="348" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="349" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="351" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="352" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="353" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="354" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="355" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="356" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="357" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="358" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="359" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="360" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="361" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="362" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="363" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="364" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="365" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="366" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="367" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="368" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="369" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="370" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="371" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="372" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="373" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3711,23 +3832,31 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:D321">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C35:C36 C306:C317 C343:C346 C319:C322">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="31">
+  <conditionalFormatting sqref="C318:C321">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C318)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C318)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations xWindow="547" yWindow="733" count="33">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3747,7 +3876,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F169" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133 C161:C162" xr:uid="{E2DEB765-B61D-AE4B-8978-020644048C29}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{E2DEB765-B61D-AE4B-8978-020644048C29}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C60 C62" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>0</formula1>
@@ -3771,6 +3900,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up for each zone" prompt="If not specified, the reserves are calculated using the method specified in the &quot;Reserve calculation&quot; variable." sqref="C161" xr:uid="{6FC56A66-A24F-44A7-9C48-DD4284F1AB32}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down for each zone" prompt="If not specified, the reserves are calculated using the method specified in the &quot;Reserve calculation&quot; variable._x000a__x000a_Unit: MW" sqref="C162" xr:uid="{45CD16F4-BF10-49AB-9071-3179C255DC54}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3781,7 +3912,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C226:D247 F226:G247 C306:D321</xm:sqref>
+          <xm:sqref>C226:D247 F226:G247 C306:C322 C343:C346</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
@@ -3843,19 +3974,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3875,7 +4006,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3895,13 +4026,16 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
       <c r="D3" t="s">
         <v>84</v>
       </c>
@@ -3912,10 +4046,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>45</v>
       </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
       <c r="D4" t="s">
         <v>81</v>
       </c>
@@ -3923,15 +4060,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>133</v>
       </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
       <c r="D5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3951,12 +4091,12 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
@@ -4000,7 +4140,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -4047,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -4094,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>94</v>
       </c>
@@ -4141,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
@@ -4188,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
@@ -4235,7 +4375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>97</v>
       </c>
@@ -4282,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
@@ -4329,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>99</v>
       </c>
@@ -4376,7 +4516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>100</v>
       </c>
@@ -4423,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -4470,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -4517,7 +4657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
@@ -4564,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>104</v>
       </c>
@@ -4611,7 +4751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>105</v>
       </c>
@@ -4658,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>106</v>
       </c>

</xml_diff>